<commit_message>
some notes for the writeup
</commit_message>
<xml_diff>
--- a/Practical2/solution/practical2-code/bb.xlsx
+++ b/Practical2/solution/practical2-code/bb.xlsx
@@ -4,11 +4,39 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10580" yWindow="1520" windowWidth="25040" windowHeight="18460" tabRatio="500"/>
+    <workbookView xWindow="7480" yWindow="1380" windowWidth="25040" windowHeight="18460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="bb.txt" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">bb.txt!$M$2:$M$3</definedName>
+    <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_lin" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">bb.txt!$H$1151</definedName>
+    <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="0" hidden="1">2</definedName>
+  </definedNames>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -459,15 +487,15 @@
   <dimension ref="A1:M1151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6880" topLeftCell="A1139"/>
-      <selection activeCell="M2" sqref="M2"/>
-      <selection pane="bottomLeft" activeCell="G232" sqref="G232"/>
+      <pane ySplit="6880" topLeftCell="A1139" activePane="bottomLeft"/>
+      <selection activeCell="H2" sqref="H2"/>
+      <selection pane="bottomLeft" activeCell="D1152" sqref="D1152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="4" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.83203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="18.83203125" customWidth="1"/>
     <col min="8" max="8" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
@@ -528,7 +556,7 @@
         <v>901500.62735405297</v>
       </c>
       <c r="M2">
-        <v>0.7</v>
+        <v>0.85184917551604855</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -701,11 +729,11 @@
       </c>
       <c r="G8" s="1">
         <f t="shared" si="1"/>
-        <v>18059122.027971849</v>
+        <v>21976640.300102189</v>
       </c>
       <c r="H8" s="1">
         <f t="shared" si="2"/>
-        <v>52826178.972028151</v>
+        <v>48908660.699897811</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -1078,11 +1106,11 @@
       </c>
       <c r="G21" s="1">
         <f t="shared" si="1"/>
-        <v>11033860.58818155</v>
+        <v>13427407.206859251</v>
       </c>
       <c r="H21" s="1">
         <f t="shared" si="2"/>
-        <v>1627251.4118184503</v>
+        <v>766295.20685925148</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -1281,11 +1309,11 @@
       </c>
       <c r="G28" s="1">
         <f t="shared" si="1"/>
-        <v>5187504.2356987707</v>
+        <v>6312816.0088085821</v>
       </c>
       <c r="H28" s="1">
         <f t="shared" si="2"/>
-        <v>1515138.2356987707</v>
+        <v>2640450.0088085821</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1426,11 +1454,11 @@
       </c>
       <c r="G33" s="1">
         <f t="shared" si="1"/>
-        <v>25227319.619991016</v>
+        <v>30699816.312527407</v>
       </c>
       <c r="H33" s="1">
         <f t="shared" si="2"/>
-        <v>19080097.380008984</v>
+        <v>13607600.687472593</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1571,11 +1599,11 @@
       </c>
       <c r="G38" s="1">
         <f t="shared" si="1"/>
-        <v>20471792.011175048</v>
+        <v>24912684.494364996</v>
       </c>
       <c r="H38" s="1">
         <f t="shared" si="2"/>
-        <v>23093342.988824952</v>
+        <v>18652450.505635004</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -2180,11 +2208,11 @@
       </c>
       <c r="G59" s="1">
         <f t="shared" si="1"/>
-        <v>10090249.38191333</v>
+        <v>12279100.881048841</v>
       </c>
       <c r="H59" s="1">
         <f t="shared" si="2"/>
-        <v>5795313.3819133304</v>
+        <v>7984164.8810488414</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -2905,11 +2933,11 @@
       </c>
       <c r="G84" s="1">
         <f t="shared" si="4"/>
-        <v>21249242.999427166</v>
+        <v>25858785.899146002</v>
       </c>
       <c r="H84" s="1">
         <f t="shared" si="5"/>
-        <v>5428378.9994271658</v>
+        <v>10037921.899146002</v>
       </c>
     </row>
     <row r="85" spans="1:8">
@@ -2934,11 +2962,11 @@
       </c>
       <c r="G85" s="1">
         <f t="shared" si="4"/>
-        <v>6284371.5314149698</v>
+        <v>7647623.868103385</v>
       </c>
       <c r="H85" s="1">
         <f t="shared" si="5"/>
-        <v>3082951.5314149698</v>
+        <v>4446203.868103385</v>
       </c>
     </row>
     <row r="86" spans="1:8">
@@ -2963,11 +2991,11 @@
       </c>
       <c r="G86" s="1">
         <f t="shared" si="4"/>
-        <v>43688379.750132598</v>
+        <v>53165586.099689268</v>
       </c>
       <c r="H86" s="1">
         <f t="shared" si="5"/>
-        <v>29208606.249867402</v>
+        <v>19731399.900310732</v>
       </c>
     </row>
     <row r="87" spans="1:8">
@@ -3253,11 +3281,11 @@
       </c>
       <c r="G96" s="1">
         <f t="shared" si="4"/>
-        <v>21302638.86130324</v>
+        <v>25923764.786167573</v>
       </c>
       <c r="H96" s="1">
         <f t="shared" si="5"/>
-        <v>2147573.1386967599</v>
+        <v>2473552.7861675732</v>
       </c>
     </row>
     <row r="97" spans="1:8">
@@ -3282,11 +3310,11 @@
       </c>
       <c r="G97" s="1">
         <f t="shared" si="4"/>
-        <v>46043743.867943287</v>
+        <v>56031893.216542296</v>
       </c>
       <c r="H97" s="1">
         <f t="shared" si="5"/>
-        <v>8022699.8679432869</v>
+        <v>18010849.216542296</v>
       </c>
     </row>
     <row r="98" spans="1:8">
@@ -3659,11 +3687,11 @@
       </c>
       <c r="G110" s="1">
         <f t="shared" si="4"/>
-        <v>26194744.167841196</v>
+        <v>31877101.746041924</v>
       </c>
       <c r="H110" s="1">
         <f t="shared" si="5"/>
-        <v>1321126.8321588039</v>
+        <v>4361230.7460419238</v>
       </c>
     </row>
     <row r="111" spans="1:8">
@@ -3717,11 +3745,11 @@
       </c>
       <c r="G112" s="1">
         <f t="shared" si="4"/>
-        <v>20924951.807173047</v>
+        <v>25464147.06379059</v>
       </c>
       <c r="H112" s="1">
         <f t="shared" si="5"/>
-        <v>793821.80717304721</v>
+        <v>5333017.0637905896</v>
       </c>
     </row>
     <row r="113" spans="1:8">
@@ -3949,11 +3977,11 @@
       </c>
       <c r="G120" s="1">
         <f t="shared" si="4"/>
-        <v>8342298.8713256503</v>
+        <v>10151972.022067454</v>
       </c>
       <c r="H120" s="1">
         <f t="shared" si="5"/>
-        <v>1663596.1286743497</v>
+        <v>146077.02206745371</v>
       </c>
     </row>
     <row r="121" spans="1:8">
@@ -4036,11 +4064,11 @@
       </c>
       <c r="G123" s="1">
         <f t="shared" si="4"/>
-        <v>23354195.704321019</v>
+        <v>28420360.507951863</v>
       </c>
       <c r="H123" s="1">
         <f t="shared" si="5"/>
-        <v>9660006.2956789806</v>
+        <v>4593841.4920481369</v>
       </c>
     </row>
     <row r="124" spans="1:8">
@@ -4152,11 +4180,11 @@
       </c>
       <c r="G127" s="1">
         <f t="shared" si="4"/>
-        <v>9967243.0581054091</v>
+        <v>12129411.116021644</v>
       </c>
       <c r="H127" s="1">
         <f t="shared" si="5"/>
-        <v>1318919.0581054091</v>
+        <v>3481087.1160216443</v>
       </c>
     </row>
     <row r="128" spans="1:8">
@@ -4413,11 +4441,11 @@
       </c>
       <c r="G136" s="1">
         <f t="shared" si="7"/>
-        <v>36072965.593624115</v>
+        <v>43898179.999067843</v>
       </c>
       <c r="H136" s="1">
         <f t="shared" si="8"/>
-        <v>33210724.406375885</v>
+        <v>25385510.000932157</v>
       </c>
     </row>
     <row r="137" spans="1:8">
@@ -4703,11 +4731,11 @@
       </c>
       <c r="G146" s="1">
         <f t="shared" si="7"/>
-        <v>16860183.63437324</v>
+        <v>20517619.32570003</v>
       </c>
       <c r="H146" s="1">
         <f t="shared" si="8"/>
-        <v>22312601.36562676</v>
+        <v>18655165.67429997</v>
       </c>
     </row>
     <row r="147" spans="1:8">
@@ -5109,11 +5137,11 @@
       </c>
       <c r="G160" s="1">
         <f t="shared" si="7"/>
-        <v>19402596.847653247</v>
+        <v>23611551.610776719</v>
       </c>
       <c r="H160" s="1">
         <f t="shared" si="8"/>
-        <v>4310517.8476532474</v>
+        <v>8519472.6107767187</v>
       </c>
     </row>
     <row r="161" spans="1:8">
@@ -5573,11 +5601,11 @@
       </c>
       <c r="G176" s="1">
         <f t="shared" si="7"/>
-        <v>41601094.163069554</v>
+        <v>50625511.090537578</v>
       </c>
       <c r="H176" s="1">
         <f t="shared" si="8"/>
-        <v>18518414.836930446</v>
+        <v>9493997.9094624221</v>
       </c>
     </row>
     <row r="177" spans="1:8">
@@ -5631,11 +5659,11 @@
       </c>
       <c r="G178" s="1">
         <f t="shared" si="7"/>
-        <v>28056286.31401379</v>
+        <v>34142463.378049776</v>
       </c>
       <c r="H178" s="1">
         <f t="shared" si="8"/>
-        <v>12776869.68598621</v>
+        <v>6690692.621950224</v>
       </c>
     </row>
     <row r="179" spans="1:8">
@@ -5892,11 +5920,11 @@
       </c>
       <c r="G187" s="1">
         <f t="shared" si="7"/>
-        <v>40903834.782093845</v>
+        <v>49776997.049387589</v>
       </c>
       <c r="H187" s="1">
         <f t="shared" si="8"/>
-        <v>15274615.217906155</v>
+        <v>6401452.9506124109</v>
       </c>
     </row>
     <row r="188" spans="1:8">
@@ -5921,11 +5949,11 @@
       </c>
       <c r="G188" s="1">
         <f t="shared" si="7"/>
-        <v>12320306.810890401</v>
+        <v>14992918.855659636</v>
       </c>
       <c r="H188" s="1">
         <f t="shared" si="8"/>
-        <v>2664056.8108904008</v>
+        <v>5336668.8556596357</v>
       </c>
     </row>
     <row r="189" spans="1:8">
@@ -5950,11 +5978,11 @@
       </c>
       <c r="G189" s="1">
         <f t="shared" si="7"/>
-        <v>29711180.350122947</v>
+        <v>36156349.264086939</v>
       </c>
       <c r="H189" s="1">
         <f t="shared" si="8"/>
-        <v>18253827.350122947</v>
+        <v>24698996.264086939</v>
       </c>
     </row>
     <row r="190" spans="1:8">
@@ -5979,11 +6007,11 @@
       </c>
       <c r="G190" s="1">
         <f t="shared" si="7"/>
-        <v>19329214.270596437</v>
+        <v>23522250.34254374</v>
       </c>
       <c r="H190" s="1">
         <f t="shared" si="8"/>
-        <v>4738073.2705964372</v>
+        <v>8931109.3425437398</v>
       </c>
     </row>
     <row r="191" spans="1:8">
@@ -6008,11 +6036,11 @@
       </c>
       <c r="G191" s="1">
         <f t="shared" si="7"/>
-        <v>30256694.134500608</v>
+        <v>36820199.931879438</v>
       </c>
       <c r="H191" s="1">
         <f t="shared" si="8"/>
-        <v>9793083.8654993922</v>
+        <v>3229578.0681205615</v>
       </c>
     </row>
     <row r="192" spans="1:8">
@@ -6037,11 +6065,11 @@
       </c>
       <c r="G192" s="1">
         <f t="shared" si="7"/>
-        <v>6133126.2794923093</v>
+        <v>7463569.3778876206</v>
       </c>
       <c r="H192" s="1">
         <f t="shared" si="8"/>
-        <v>5050322.2794923093</v>
+        <v>6380765.3778876206</v>
       </c>
     </row>
     <row r="193" spans="1:8">
@@ -6182,11 +6210,11 @@
       </c>
       <c r="G197" s="1">
         <f t="shared" si="10"/>
-        <v>16015521.721894799</v>
+        <v>19489727.106079217</v>
       </c>
       <c r="H197" s="1">
         <f t="shared" si="11"/>
-        <v>2304683.2781052012</v>
+        <v>1169522.106079217</v>
       </c>
     </row>
     <row r="198" spans="1:8">
@@ -6240,11 +6268,11 @@
       </c>
       <c r="G199" s="1">
         <f t="shared" si="10"/>
-        <v>34820316.965490982</v>
+        <v>42373797.568944238</v>
       </c>
       <c r="H199" s="1">
         <f t="shared" si="11"/>
-        <v>5191048.0345090181</v>
+        <v>2362432.5689442381</v>
       </c>
     </row>
     <row r="200" spans="1:8">
@@ -6733,11 +6761,11 @@
       </c>
       <c r="G216" s="1">
         <f t="shared" si="10"/>
-        <v>17692819.485771149</v>
+        <v>21530876.702154905</v>
       </c>
       <c r="H216" s="1">
         <f t="shared" si="11"/>
-        <v>12076278.514228851</v>
+        <v>8238221.2978450954</v>
       </c>
     </row>
     <row r="217" spans="1:8">
@@ -7284,11 +7312,11 @@
       </c>
       <c r="G235" s="1">
         <f t="shared" si="10"/>
-        <v>10349371.805303019</v>
+        <v>12594434.05636631</v>
       </c>
       <c r="H235" s="1">
         <f t="shared" si="11"/>
-        <v>5462086.8053030185</v>
+        <v>7707149.0563663095</v>
       </c>
     </row>
     <row r="236" spans="1:8">
@@ -7516,11 +7544,11 @@
       </c>
       <c r="G243" s="1">
         <f t="shared" si="10"/>
-        <v>11947168.30352059</v>
+        <v>14538836.384436406</v>
       </c>
       <c r="H243" s="1">
         <f t="shared" si="11"/>
-        <v>2007917.3035205901</v>
+        <v>4599585.3844364062</v>
       </c>
     </row>
     <row r="244" spans="1:8">
@@ -7661,11 +7689,11 @@
       </c>
       <c r="G248" s="1">
         <f t="shared" si="10"/>
-        <v>37831701.90388862</v>
+        <v>46038434.393137783</v>
       </c>
       <c r="H248" s="1">
         <f t="shared" si="11"/>
-        <v>39241686.09611138</v>
+        <v>31034953.606862217</v>
       </c>
     </row>
     <row r="249" spans="1:8">
@@ -8183,11 +8211,11 @@
       </c>
       <c r="G266" s="1">
         <f t="shared" si="13"/>
-        <v>19758498.440399736</v>
+        <v>24044658.008413784</v>
       </c>
       <c r="H266" s="1">
         <f t="shared" si="14"/>
-        <v>8890899.5596002638</v>
+        <v>4604739.9915862158</v>
       </c>
     </row>
     <row r="267" spans="1:8">
@@ -8270,11 +8298,11 @@
       </c>
       <c r="G269" s="1">
         <f t="shared" si="13"/>
-        <v>19074627.44739062</v>
+        <v>23212436.663336415</v>
       </c>
       <c r="H269" s="1">
         <f t="shared" si="14"/>
-        <v>7812839.5526093803</v>
+        <v>3675030.3366635852</v>
       </c>
     </row>
     <row r="270" spans="1:8">
@@ -9053,11 +9081,11 @@
       </c>
       <c r="G296" s="1">
         <f t="shared" si="13"/>
-        <v>17873105.987290747</v>
+        <v>21750272.284549396</v>
       </c>
       <c r="H296" s="1">
         <f t="shared" si="14"/>
-        <v>2384235.9872907475</v>
+        <v>6261402.2845493965</v>
       </c>
     </row>
     <row r="297" spans="1:8">
@@ -9314,11 +9342,11 @@
       </c>
       <c r="G305" s="1">
         <f t="shared" si="13"/>
-        <v>6052427.2402903605</v>
+        <v>7365364.5064460244</v>
       </c>
       <c r="H305" s="1">
         <f t="shared" si="14"/>
-        <v>5673477.2402903605</v>
+        <v>6986414.5064460244</v>
       </c>
     </row>
     <row r="306" spans="1:8">
@@ -9430,11 +9458,11 @@
       </c>
       <c r="G309" s="1">
         <f t="shared" si="13"/>
-        <v>33537110.802960169</v>
+        <v>40812228.838131405</v>
       </c>
       <c r="H309" s="1">
         <f t="shared" si="14"/>
-        <v>2861796.8029601686</v>
+        <v>10136914.838131405</v>
       </c>
     </row>
     <row r="310" spans="1:8">
@@ -9836,11 +9864,11 @@
       </c>
       <c r="G323" s="1">
         <f t="shared" ref="G323:G386" si="16">IF(C323&gt; $M$3, E323*$M$2,E323)</f>
-        <v>20250556.653360531</v>
+        <v>24643457.127008855</v>
       </c>
       <c r="H323" s="1">
         <f t="shared" ref="H323:H386" si="17">ABS(G323-D323)</f>
-        <v>7445763.6533605307</v>
+        <v>11838664.127008855</v>
       </c>
     </row>
     <row r="324" spans="1:8">
@@ -9923,11 +9951,11 @@
       </c>
       <c r="G326" s="1">
         <f t="shared" si="16"/>
-        <v>10079704.380384449</v>
+        <v>12266268.379822852</v>
       </c>
       <c r="H326" s="1">
         <f t="shared" si="17"/>
-        <v>539006.61961555108</v>
+        <v>1647557.3798228521</v>
       </c>
     </row>
     <row r="327" spans="1:8">
@@ -10097,11 +10125,11 @@
       </c>
       <c r="G332" s="1">
         <f t="shared" si="16"/>
-        <v>34455474.784675136</v>
+        <v>41929811.124770738</v>
       </c>
       <c r="H332" s="1">
         <f t="shared" si="17"/>
-        <v>14604806.215324864</v>
+        <v>7130469.8752292618</v>
       </c>
     </row>
     <row r="333" spans="1:8">
@@ -10213,11 +10241,11 @@
       </c>
       <c r="G336" s="1">
         <f t="shared" si="16"/>
-        <v>19928668.501861978</v>
+        <v>24251742.617776822</v>
       </c>
       <c r="H336" s="1">
         <f t="shared" si="17"/>
-        <v>3311238.4981380217</v>
+        <v>1011835.6177768223</v>
       </c>
     </row>
     <row r="337" spans="1:8">
@@ -10329,11 +10357,11 @@
       </c>
       <c r="G340" s="1">
         <f t="shared" si="16"/>
-        <v>38174310.511559181</v>
+        <v>46455364.193093307</v>
       </c>
       <c r="H340" s="1">
         <f t="shared" si="17"/>
-        <v>6981695.5115591809</v>
+        <v>15262749.193093307</v>
       </c>
     </row>
     <row r="341" spans="1:8">
@@ -10764,11 +10792,11 @@
       </c>
       <c r="G355" s="1">
         <f t="shared" si="16"/>
-        <v>44706913.650022954</v>
+        <v>54405067.903770335</v>
       </c>
       <c r="H355" s="1">
         <f t="shared" si="17"/>
-        <v>13344770.349977046</v>
+        <v>3646616.096229665</v>
       </c>
     </row>
     <row r="356" spans="1:8">
@@ -10793,11 +10821,11 @@
       </c>
       <c r="G356" s="1">
         <f t="shared" si="16"/>
-        <v>31059800.299967315</v>
+        <v>37797521.824600399</v>
       </c>
       <c r="H356" s="1">
         <f t="shared" si="17"/>
-        <v>25001703.700032685</v>
+        <v>18263982.175399601</v>
       </c>
     </row>
     <row r="357" spans="1:8">
@@ -11605,11 +11633,11 @@
       </c>
       <c r="G384" s="1">
         <f t="shared" si="16"/>
-        <v>6042854.8187630698</v>
+        <v>7353715.5644664317</v>
       </c>
       <c r="H384" s="1">
         <f t="shared" si="17"/>
-        <v>4202335.1812369302</v>
+        <v>2891474.4355335683</v>
       </c>
     </row>
     <row r="385" spans="1:8">
@@ -11721,11 +11749,11 @@
       </c>
       <c r="G388" s="1">
         <f t="shared" si="19"/>
-        <v>24033512.7946277</v>
+        <v>29247040.084082872</v>
       </c>
       <c r="H388" s="1">
         <f t="shared" si="20"/>
-        <v>596425.2053723</v>
+        <v>4617102.0840828717</v>
       </c>
     </row>
     <row r="389" spans="1:8">
@@ -11750,11 +11778,11 @@
       </c>
       <c r="G389" s="1">
         <f t="shared" si="19"/>
-        <v>38945829.021564774</v>
+        <v>47394246.202584222</v>
       </c>
       <c r="H389" s="1">
         <f t="shared" si="20"/>
-        <v>20131506.021564774</v>
+        <v>28579923.202584222</v>
       </c>
     </row>
     <row r="390" spans="1:8">
@@ -11779,11 +11807,11 @@
       </c>
       <c r="G390" s="1">
         <f t="shared" si="19"/>
-        <v>7277290.8903933689</v>
+        <v>8855934.6356743462</v>
       </c>
       <c r="H390" s="1">
         <f t="shared" si="20"/>
-        <v>1273071.8903933689</v>
+        <v>2851715.6356743462</v>
       </c>
     </row>
     <row r="391" spans="1:8">
@@ -12301,11 +12329,11 @@
       </c>
       <c r="G408" s="1">
         <f t="shared" si="19"/>
-        <v>23732272.071598649</v>
+        <v>28880451.996162649</v>
       </c>
       <c r="H408" s="1">
         <f t="shared" si="20"/>
-        <v>1773001.071598649</v>
+        <v>6921180.9961626492</v>
       </c>
     </row>
     <row r="409" spans="1:8">
@@ -12678,11 +12706,11 @@
       </c>
       <c r="G421" s="1">
         <f t="shared" si="19"/>
-        <v>34138792.093909927</v>
+        <v>41544431.283301383</v>
       </c>
       <c r="H421" s="1">
         <f t="shared" si="20"/>
-        <v>11250043.906090073</v>
+        <v>3844404.7166986167</v>
       </c>
     </row>
     <row r="422" spans="1:8">
@@ -13026,11 +13054,11 @@
       </c>
       <c r="G433" s="1">
         <f t="shared" si="19"/>
-        <v>38629756.175515465</v>
+        <v>47009608.497855484</v>
       </c>
       <c r="H433" s="1">
         <f t="shared" si="20"/>
-        <v>12846524.175515465</v>
+        <v>21226376.497855484</v>
       </c>
     </row>
     <row r="434" spans="1:8">
@@ -13635,11 +13663,11 @@
       </c>
       <c r="G454" s="1">
         <f t="shared" si="22"/>
-        <v>4906084.5040348889</v>
+        <v>5970348.6282488322</v>
       </c>
       <c r="H454" s="1">
         <f t="shared" si="23"/>
-        <v>1530075.5040348889</v>
+        <v>2594339.6282488322</v>
       </c>
     </row>
     <row r="455" spans="1:8">
@@ -13722,11 +13750,11 @@
       </c>
       <c r="G457" s="1">
         <f t="shared" si="22"/>
-        <v>11035808.70160874</v>
+        <v>13429777.919454629</v>
       </c>
       <c r="H457" s="1">
         <f t="shared" si="23"/>
-        <v>560804.29839126021</v>
+        <v>1833164.9194546286</v>
       </c>
     </row>
     <row r="458" spans="1:8">
@@ -14012,11 +14040,11 @@
       </c>
       <c r="G467" s="1">
         <f t="shared" si="22"/>
-        <v>19578969.21740501</v>
+        <v>23826183.979000788</v>
       </c>
       <c r="H467" s="1">
         <f t="shared" si="23"/>
-        <v>7897775.78259499</v>
+        <v>3650561.0209992118</v>
       </c>
     </row>
     <row r="468" spans="1:8">
@@ -14244,11 +14272,11 @@
       </c>
       <c r="G475" s="1">
         <f t="shared" si="22"/>
-        <v>36711438.851592325</v>
+        <v>44675155.5967668</v>
       </c>
       <c r="H475" s="1">
         <f t="shared" si="23"/>
-        <v>4821993.1484076753</v>
+        <v>3141723.5967667997</v>
       </c>
     </row>
     <row r="476" spans="1:8">
@@ -14360,11 +14388,11 @@
       </c>
       <c r="G479" s="1">
         <f t="shared" si="22"/>
-        <v>43688379.750132598</v>
+        <v>53165586.099689268</v>
       </c>
       <c r="H479" s="1">
         <f t="shared" si="23"/>
-        <v>58646686.249867402</v>
+        <v>49169479.900310732</v>
       </c>
     </row>
     <row r="480" spans="1:8">
@@ -14389,11 +14417,11 @@
       </c>
       <c r="G480" s="1">
         <f t="shared" si="22"/>
-        <v>60168312.635840632</v>
+        <v>73220467.872903839</v>
       </c>
       <c r="H480" s="1">
         <f t="shared" si="23"/>
-        <v>79546844.364159375</v>
+        <v>66494689.127096161</v>
       </c>
     </row>
     <row r="481" spans="1:8">
@@ -15143,11 +15171,11 @@
       </c>
       <c r="G506" s="1">
         <f t="shared" si="22"/>
-        <v>27725572.72162769</v>
+        <v>33740008.948041134</v>
       </c>
       <c r="H506" s="1">
         <f t="shared" si="23"/>
-        <v>15416641.27837231</v>
+        <v>9402205.0519588664</v>
       </c>
     </row>
     <row r="507" spans="1:8">
@@ -15230,11 +15258,11 @@
       </c>
       <c r="G509" s="1">
         <f t="shared" si="22"/>
-        <v>13475086.09955053</v>
+        <v>16398201.405585552</v>
       </c>
       <c r="H509" s="1">
         <f t="shared" si="23"/>
-        <v>696173.09955053031</v>
+        <v>3619288.4055855516</v>
       </c>
     </row>
     <row r="510" spans="1:8">
@@ -15491,11 +15519,11 @@
       </c>
       <c r="G518" s="1">
         <f t="shared" si="25"/>
-        <v>8948514.79011406</v>
+        <v>10889692.780074039</v>
       </c>
       <c r="H518" s="1">
         <f t="shared" si="26"/>
-        <v>1266219.20988594</v>
+        <v>674958.78007403947</v>
       </c>
     </row>
     <row r="519" spans="1:8">
@@ -15926,11 +15954,11 @@
       </c>
       <c r="G533" s="1">
         <f t="shared" si="25"/>
-        <v>36210268.746516615</v>
+        <v>44065267.967049606</v>
       </c>
       <c r="H533" s="1">
         <f t="shared" si="26"/>
-        <v>41001052.253483385</v>
+        <v>33146053.032950394</v>
       </c>
     </row>
     <row r="534" spans="1:8">
@@ -15955,11 +15983,11 @@
       </c>
       <c r="G534" s="1">
         <f t="shared" si="25"/>
-        <v>41252721.434155561</v>
+        <v>50201566.773540914</v>
       </c>
       <c r="H534" s="1">
         <f t="shared" si="26"/>
-        <v>26780822.565844439</v>
+        <v>17831977.226459086</v>
       </c>
     </row>
     <row r="535" spans="1:8">
@@ -16448,11 +16476,11 @@
       </c>
       <c r="G551" s="1">
         <f t="shared" si="25"/>
-        <v>28131030.88733273</v>
+        <v>34233422.096844122</v>
       </c>
       <c r="H551" s="1">
         <f t="shared" si="26"/>
-        <v>6102719.11266727</v>
+        <v>327.90315587818623</v>
       </c>
     </row>
     <row r="552" spans="1:8">
@@ -16535,11 +16563,11 @@
       </c>
       <c r="G554" s="1">
         <f t="shared" si="25"/>
-        <v>15511674.387113517</v>
+        <v>18876581.482194372</v>
       </c>
       <c r="H554" s="1">
         <f t="shared" si="26"/>
-        <v>7310780.6128864828</v>
+        <v>3945873.5178056285</v>
       </c>
     </row>
     <row r="555" spans="1:8">
@@ -16738,11 +16766,11 @@
       </c>
       <c r="G561" s="1">
         <f t="shared" si="25"/>
-        <v>14922142.533537399</v>
+        <v>18159164.020181134</v>
       </c>
       <c r="H561" s="1">
         <f t="shared" si="26"/>
-        <v>8970733.533537399</v>
+        <v>12207755.020181134</v>
       </c>
     </row>
     <row r="562" spans="1:8">
@@ -16854,11 +16882,11 @@
       </c>
       <c r="G565" s="1">
         <f t="shared" si="25"/>
-        <v>23227770.059396628</v>
+        <v>28266509.677390542</v>
       </c>
       <c r="H565" s="1">
         <f t="shared" si="26"/>
-        <v>10818700.059396628</v>
+        <v>15857439.677390542</v>
       </c>
     </row>
     <row r="566" spans="1:8">
@@ -17086,11 +17114,11 @@
       </c>
       <c r="G573" s="1">
         <f t="shared" si="25"/>
-        <v>10627595.303115349</v>
+        <v>12933011.852395773</v>
       </c>
       <c r="H573" s="1">
         <f t="shared" si="26"/>
-        <v>17098614.696884651</v>
+        <v>14793198.147604227</v>
       </c>
     </row>
     <row r="574" spans="1:8">
@@ -17463,11 +17491,11 @@
       </c>
       <c r="G586" s="1">
         <f t="shared" si="28"/>
-        <v>26270414.797209799</v>
+        <v>31969187.407811098</v>
       </c>
       <c r="H586" s="1">
         <f t="shared" si="29"/>
-        <v>9861696.7972097993</v>
+        <v>15560469.407811098</v>
       </c>
     </row>
     <row r="587" spans="1:8">
@@ -17753,11 +17781,11 @@
       </c>
       <c r="G596" s="1">
         <f t="shared" si="28"/>
-        <v>24127104.906766675</v>
+        <v>29360934.889169149</v>
       </c>
       <c r="H596" s="1">
         <f t="shared" si="29"/>
-        <v>4491108.9067666754</v>
+        <v>9724938.8891691491</v>
       </c>
     </row>
     <row r="597" spans="1:8">
@@ -17782,11 +17810,11 @@
       </c>
       <c r="G597" s="1">
         <f t="shared" si="28"/>
-        <v>14526198.415732428</v>
+        <v>17677328.776891716</v>
       </c>
       <c r="H597" s="1">
         <f t="shared" si="29"/>
-        <v>2608856.5842675716</v>
+        <v>542273.77689171582</v>
       </c>
     </row>
     <row r="598" spans="1:8">
@@ -17811,11 +17839,11 @@
       </c>
       <c r="G598" s="1">
         <f t="shared" si="28"/>
-        <v>39809971.570257142</v>
+        <v>48445844.942058399</v>
       </c>
       <c r="H598" s="1">
         <f t="shared" si="29"/>
-        <v>26371673.429742858</v>
+        <v>17735800.057941601</v>
       </c>
     </row>
     <row r="599" spans="1:8">
@@ -18246,11 +18274,11 @@
       </c>
       <c r="G613" s="1">
         <f t="shared" si="28"/>
-        <v>21666235.791829649</v>
+        <v>26366235.851151984</v>
       </c>
       <c r="H613" s="1">
         <f t="shared" si="29"/>
-        <v>3621839.7918296494</v>
+        <v>8321839.8511519842</v>
       </c>
     </row>
     <row r="614" spans="1:8">
@@ -18710,11 +18738,11 @@
       </c>
       <c r="G629" s="1">
         <f t="shared" si="28"/>
-        <v>7697006.4840459693</v>
+        <v>9366698.0391089134</v>
       </c>
       <c r="H629" s="1">
         <f t="shared" si="29"/>
-        <v>4950694.4840459693</v>
+        <v>6620386.0391089134</v>
       </c>
     </row>
     <row r="630" spans="1:8">
@@ -18884,11 +18912,11 @@
       </c>
       <c r="G635" s="1">
         <f t="shared" si="28"/>
-        <v>28342727.15095045</v>
+        <v>34491041.079162091</v>
       </c>
       <c r="H635" s="1">
         <f t="shared" si="29"/>
-        <v>12014221.15095045</v>
+        <v>18162535.079162091</v>
       </c>
     </row>
     <row r="636" spans="1:8">
@@ -19116,11 +19144,11 @@
       </c>
       <c r="G643" s="1">
         <f t="shared" ref="G643:G706" si="31">IF(C643&gt; $M$3, E643*$M$2,E643)</f>
-        <v>38899746.26359906</v>
+        <v>47338166.832043357</v>
       </c>
       <c r="H643" s="1">
         <f t="shared" ref="H643:H706" si="32">ABS(G643-D643)</f>
-        <v>26656565.73640094</v>
+        <v>18218145.167956643</v>
       </c>
     </row>
     <row r="644" spans="1:8">
@@ -19203,11 +19231,11 @@
       </c>
       <c r="G646" s="1">
         <f t="shared" si="31"/>
-        <v>11033580.606892409</v>
+        <v>13427066.489958802</v>
       </c>
       <c r="H646" s="1">
         <f t="shared" si="32"/>
-        <v>10579595.393107591</v>
+        <v>8186109.5100411978</v>
       </c>
     </row>
     <row r="647" spans="1:8">
@@ -19290,11 +19318,11 @@
       </c>
       <c r="G649" s="1">
         <f t="shared" si="31"/>
-        <v>28108255.79386111</v>
+        <v>34205706.461706832</v>
       </c>
       <c r="H649" s="1">
         <f t="shared" si="32"/>
-        <v>20289874.20613889</v>
+        <v>14192423.538293168</v>
       </c>
     </row>
     <row r="650" spans="1:8">
@@ -19464,11 +19492,11 @@
       </c>
       <c r="G655" s="1">
         <f t="shared" si="31"/>
-        <v>31480198.615710109</v>
+        <v>38309116.051248729</v>
       </c>
       <c r="H655" s="1">
         <f t="shared" si="32"/>
-        <v>16126281.384289891</v>
+        <v>9297363.9487512708</v>
       </c>
     </row>
     <row r="656" spans="1:8">
@@ -19841,11 +19869,11 @@
       </c>
       <c r="G668" s="1">
         <f t="shared" si="31"/>
-        <v>10233497.341208609</v>
+        <v>12453423.246791756</v>
       </c>
       <c r="H668" s="1">
         <f t="shared" si="32"/>
-        <v>7523052.3412086088</v>
+        <v>9742978.2467917558</v>
       </c>
     </row>
     <row r="669" spans="1:8">
@@ -19928,11 +19956,11 @@
       </c>
       <c r="G671" s="1">
         <f t="shared" si="31"/>
-        <v>47570051.088763908</v>
+        <v>57889298.284599781</v>
       </c>
       <c r="H671" s="1">
         <f t="shared" si="32"/>
-        <v>345457.08876390755</v>
+        <v>10664704.284599781</v>
       </c>
     </row>
     <row r="672" spans="1:8">
@@ -20682,11 +20710,11 @@
       </c>
       <c r="G697" s="1">
         <f t="shared" si="31"/>
-        <v>6859417.5395665988</v>
+        <v>8347413.1080001853</v>
       </c>
       <c r="H697" s="1">
         <f t="shared" si="32"/>
-        <v>6176913.5395665988</v>
+        <v>7664909.1080001853</v>
       </c>
     </row>
     <row r="698" spans="1:8">
@@ -20769,11 +20797,11 @@
       </c>
       <c r="G700" s="1">
         <f t="shared" si="31"/>
-        <v>22768849.324716806</v>
+        <v>27708036.46387022</v>
       </c>
       <c r="H700" s="1">
         <f t="shared" si="32"/>
-        <v>2954965.6752831936</v>
+        <v>1984221.4638702199</v>
       </c>
     </row>
     <row r="701" spans="1:8">
@@ -21059,11 +21087,11 @@
       </c>
       <c r="G710" s="1">
         <f t="shared" si="34"/>
-        <v>20417173.935876898</v>
+        <v>24846218.262349274</v>
       </c>
       <c r="H710" s="1">
         <f t="shared" si="35"/>
-        <v>3318654.9358768985</v>
+        <v>7747699.262349274</v>
       </c>
     </row>
     <row r="711" spans="1:8">
@@ -21088,11 +21116,11 @@
       </c>
       <c r="G711" s="1">
         <f t="shared" si="34"/>
-        <v>50612475.358928479</v>
+        <v>61591707.72189936</v>
       </c>
       <c r="H711" s="1">
         <f t="shared" si="35"/>
-        <v>2869202.3589284793</v>
+        <v>13848434.72189936</v>
       </c>
     </row>
     <row r="712" spans="1:8">
@@ -21291,11 +21319,11 @@
       </c>
       <c r="G718" s="1">
         <f t="shared" si="34"/>
-        <v>28771601.355602279</v>
+        <v>35012949.847208895</v>
       </c>
       <c r="H718" s="1">
         <f t="shared" si="35"/>
-        <v>6554375.3556022793</v>
+        <v>12795723.847208895</v>
       </c>
     </row>
     <row r="719" spans="1:8">
@@ -21436,11 +21464,11 @@
       </c>
       <c r="G723" s="1">
         <f t="shared" si="34"/>
-        <v>28471959.437498849</v>
+        <v>34648307.388799675</v>
       </c>
       <c r="H723" s="1">
         <f t="shared" si="35"/>
-        <v>21870918.562501151</v>
+        <v>15694570.611200325</v>
       </c>
     </row>
     <row r="724" spans="1:8">
@@ -21639,11 +21667,11 @@
       </c>
       <c r="G730" s="1">
         <f t="shared" si="34"/>
-        <v>6063847.0334721506</v>
+        <v>7379261.5655981265</v>
       </c>
       <c r="H730" s="1">
         <f t="shared" si="35"/>
-        <v>1911587.0334721506</v>
+        <v>3227001.5655981265</v>
       </c>
     </row>
     <row r="731" spans="1:8">
@@ -22451,11 +22479,11 @@
       </c>
       <c r="G758" s="1">
         <f t="shared" si="34"/>
-        <v>35165143.436943099</v>
+        <v>42793426.348090813</v>
       </c>
       <c r="H758" s="1">
         <f t="shared" si="35"/>
-        <v>4731362.4369430989</v>
+        <v>12359645.348090813</v>
       </c>
     </row>
     <row r="759" spans="1:8">
@@ -22973,11 +23001,11 @@
       </c>
       <c r="G776" s="1">
         <f t="shared" si="37"/>
-        <v>29887079.562505618</v>
+        <v>36370405.834147081</v>
       </c>
       <c r="H776" s="1">
         <f t="shared" si="38"/>
-        <v>6246323.4374943823</v>
+        <v>237002.83414708078</v>
       </c>
     </row>
     <row r="777" spans="1:8">
@@ -23205,11 +23233,11 @@
       </c>
       <c r="G784" s="1">
         <f t="shared" si="37"/>
-        <v>5245436.9416640727</v>
+        <v>6383315.9056828059</v>
       </c>
       <c r="H784" s="1">
         <f t="shared" si="38"/>
-        <v>5176989.9416640727</v>
+        <v>6314868.9056828059</v>
       </c>
     </row>
     <row r="785" spans="1:8">
@@ -23466,11 +23494,11 @@
       </c>
       <c r="G793" s="1">
         <f t="shared" si="37"/>
-        <v>37632215.605018578</v>
+        <v>45795674.051396079</v>
       </c>
       <c r="H793" s="1">
         <f t="shared" si="38"/>
-        <v>14007667.605018578</v>
+        <v>22171126.051396079</v>
       </c>
     </row>
     <row r="794" spans="1:8">
@@ -23756,11 +23784,11 @@
       </c>
       <c r="G803" s="1">
         <f t="shared" si="37"/>
-        <v>18219884.273648538</v>
+        <v>22172276.280721899</v>
       </c>
       <c r="H803" s="1">
         <f t="shared" si="38"/>
-        <v>12332809.726351462</v>
+        <v>8380417.7192781009</v>
       </c>
     </row>
     <row r="804" spans="1:8">
@@ -24075,11 +24103,11 @@
       </c>
       <c r="G814" s="1">
         <f t="shared" si="37"/>
-        <v>5140528.2027550209</v>
+        <v>6255649.5874769427</v>
       </c>
       <c r="H814" s="1">
         <f t="shared" si="38"/>
-        <v>5083083.2027550209</v>
+        <v>6198204.5874769427</v>
       </c>
     </row>
     <row r="815" spans="1:8">
@@ -24133,11 +24161,11 @@
       </c>
       <c r="G816" s="1">
         <f t="shared" si="37"/>
-        <v>27292695.97588513</v>
+        <v>33213229.378097035</v>
       </c>
       <c r="H816" s="1">
         <f t="shared" si="38"/>
-        <v>7072283.9758851305</v>
+        <v>12992817.378097035</v>
       </c>
     </row>
     <row r="817" spans="1:8">
@@ -24162,11 +24190,11 @@
       </c>
       <c r="G817" s="1">
         <f t="shared" si="37"/>
-        <v>75822144.671814099</v>
+        <v>92270044.892204851</v>
       </c>
       <c r="H817" s="1">
         <f t="shared" si="38"/>
-        <v>52150719.328185901</v>
+        <v>35702819.107795149</v>
       </c>
     </row>
     <row r="818" spans="1:8">
@@ -24191,11 +24219,11 @@
       </c>
       <c r="G818" s="1">
         <f t="shared" si="37"/>
-        <v>59755366.057069965</v>
+        <v>72717941.869106755</v>
       </c>
       <c r="H818" s="1">
         <f t="shared" si="38"/>
-        <v>75879187.942930043</v>
+        <v>62916612.130893245</v>
       </c>
     </row>
     <row r="819" spans="1:8">
@@ -24278,11 +24306,11 @@
       </c>
       <c r="G821" s="1">
         <f t="shared" si="37"/>
-        <v>35682217.013146549</v>
+        <v>43422667.347476587</v>
       </c>
       <c r="H821" s="1">
         <f t="shared" si="38"/>
-        <v>13526807.013146549</v>
+        <v>21267257.347476587</v>
       </c>
     </row>
     <row r="822" spans="1:8">
@@ -25003,11 +25031,11 @@
       </c>
       <c r="G846" s="1">
         <f t="shared" si="40"/>
-        <v>13870577.007706089</v>
+        <v>16879485.125637561</v>
       </c>
       <c r="H846" s="1">
         <f t="shared" si="41"/>
-        <v>12671131.992293911</v>
+        <v>9662223.8743624389</v>
       </c>
     </row>
     <row r="847" spans="1:8">
@@ -25206,11 +25234,11 @@
       </c>
       <c r="G853" s="1">
         <f t="shared" si="40"/>
-        <v>46460380.089799479</v>
+        <v>56538909.24808275</v>
       </c>
       <c r="H853" s="1">
         <f t="shared" si="41"/>
-        <v>567014.91020052135</v>
+        <v>9511514.2480827495</v>
       </c>
     </row>
     <row r="854" spans="1:8">
@@ -25931,11 +25959,11 @@
       </c>
       <c r="G878" s="1">
         <f t="shared" si="40"/>
-        <v>35438676.510734983</v>
+        <v>43126296.238642216</v>
       </c>
       <c r="H878" s="1">
         <f t="shared" si="41"/>
-        <v>606624.48926501721</v>
+        <v>7080995.2386422157</v>
       </c>
     </row>
     <row r="879" spans="1:8">
@@ -26308,11 +26336,11 @@
       </c>
       <c r="G891" s="1">
         <f t="shared" si="40"/>
-        <v>43570032.440158069</v>
+        <v>53021566.016223058</v>
       </c>
       <c r="H891" s="1">
         <f t="shared" si="41"/>
-        <v>5530125.5598419309</v>
+        <v>3921408.0162230581</v>
       </c>
     </row>
     <row r="892" spans="1:8">
@@ -26395,11 +26423,11 @@
       </c>
       <c r="G894" s="1">
         <f t="shared" si="40"/>
-        <v>25809132.423744038</v>
+        <v>31407840.251358394</v>
       </c>
       <c r="H894" s="1">
         <f t="shared" si="41"/>
-        <v>7740760.4237440377</v>
+        <v>13339468.251358394</v>
       </c>
     </row>
     <row r="895" spans="1:8">
@@ -27178,11 +27206,11 @@
       </c>
       <c r="G921" s="1">
         <f t="shared" si="43"/>
-        <v>13883426.40684307</v>
+        <v>16895121.911438581</v>
       </c>
       <c r="H921" s="1">
         <f t="shared" si="44"/>
-        <v>484427.59315693006</v>
+        <v>2527267.9114385806</v>
       </c>
     </row>
     <row r="922" spans="1:8">
@@ -27468,11 +27496,11 @@
       </c>
       <c r="G931" s="1">
         <f t="shared" si="43"/>
-        <v>26260002.884803031</v>
+        <v>31956516.866383597</v>
       </c>
       <c r="H931" s="1">
         <f t="shared" si="44"/>
-        <v>9949944.8848030306</v>
+        <v>15646458.866383597</v>
       </c>
     </row>
     <row r="932" spans="1:8">
@@ -27671,11 +27699,11 @@
       </c>
       <c r="G938" s="1">
         <f t="shared" si="43"/>
-        <v>13680112.31858201</v>
+        <v>16647703.427930035</v>
       </c>
       <c r="H938" s="1">
         <f t="shared" si="44"/>
-        <v>843458.68141799048</v>
+        <v>2124132.4279300347</v>
       </c>
     </row>
     <row r="939" spans="1:8">
@@ -27758,11 +27786,11 @@
       </c>
       <c r="G941" s="1">
         <f t="shared" si="43"/>
-        <v>54068839.936716005</v>
+        <v>65797852.458858185</v>
       </c>
       <c r="H941" s="1">
         <f t="shared" si="44"/>
-        <v>68467769.063283995</v>
+        <v>56738756.541141815</v>
       </c>
     </row>
     <row r="942" spans="1:8">
@@ -27874,11 +27902,11 @@
       </c>
       <c r="G945" s="1">
         <f t="shared" si="43"/>
-        <v>39582677.771988675</v>
+        <v>48169244.8925514</v>
       </c>
       <c r="H945" s="1">
         <f t="shared" si="44"/>
-        <v>34454109.228011325</v>
+        <v>25867542.1074486</v>
       </c>
     </row>
     <row r="946" spans="1:8">
@@ -28077,11 +28105,11 @@
       </c>
       <c r="G952" s="1">
         <f t="shared" si="43"/>
-        <v>14994985.525097197</v>
+        <v>18247808.652041614</v>
       </c>
       <c r="H952" s="1">
         <f t="shared" si="44"/>
-        <v>363201.52509719692</v>
+        <v>3616024.6520416141</v>
       </c>
     </row>
     <row r="953" spans="1:8">
@@ -28570,11 +28598,11 @@
       </c>
       <c r="G969" s="1">
         <f t="shared" si="46"/>
-        <v>19102971.03397676</v>
+        <v>23246928.750285801</v>
       </c>
       <c r="H969" s="1">
         <f t="shared" si="47"/>
-        <v>11591296.03397676</v>
+        <v>15735253.750285801</v>
       </c>
     </row>
     <row r="970" spans="1:8">
@@ -28628,11 +28656,11 @@
       </c>
       <c r="G971" s="1">
         <f t="shared" si="46"/>
-        <v>6519130.4327366063</v>
+        <v>7933308.4060117994</v>
       </c>
       <c r="H971" s="1">
         <f t="shared" si="47"/>
-        <v>5601732.4327366063</v>
+        <v>7015910.4060117994</v>
       </c>
     </row>
     <row r="972" spans="1:8">
@@ -28686,11 +28714,11 @@
       </c>
       <c r="G973" s="1">
         <f t="shared" si="46"/>
-        <v>67420222.734125584</v>
+        <v>82045515.927390337</v>
       </c>
       <c r="H973" s="1">
         <f t="shared" si="47"/>
-        <v>83696293.265874416</v>
+        <v>69071000.072609663</v>
       </c>
     </row>
     <row r="974" spans="1:8">
@@ -28773,11 +28801,11 @@
       </c>
       <c r="G976" s="1">
         <f t="shared" si="46"/>
-        <v>11582918.898068629</v>
+        <v>14095571.304841457</v>
       </c>
       <c r="H976" s="1">
         <f t="shared" si="47"/>
-        <v>2413139.8980686292</v>
+        <v>4925792.3048414569</v>
       </c>
     </row>
     <row r="977" spans="1:8">
@@ -28976,11 +29004,11 @@
       </c>
       <c r="G983" s="1">
         <f t="shared" si="46"/>
-        <v>32408079.470463127</v>
+        <v>39438279.681389421</v>
       </c>
       <c r="H983" s="1">
         <f t="shared" si="47"/>
-        <v>19156534.470463127</v>
+        <v>26186734.681389421</v>
       </c>
     </row>
     <row r="984" spans="1:8">
@@ -29527,11 +29555,11 @@
       </c>
       <c r="G1002" s="1">
         <f t="shared" si="46"/>
-        <v>57649441.550316416</v>
+        <v>70155184.647996679</v>
       </c>
       <c r="H1002" s="1">
         <f t="shared" si="47"/>
-        <v>26944098.449683584</v>
+        <v>14438355.352003321</v>
       </c>
     </row>
     <row r="1003" spans="1:8">
@@ -29556,11 +29584,11 @@
       </c>
       <c r="G1003" s="1">
         <f t="shared" si="46"/>
-        <v>30156358.039125144</v>
+        <v>36698098.188850746</v>
       </c>
       <c r="H1003" s="1">
         <f t="shared" si="47"/>
-        <v>12516109.039125144</v>
+        <v>19057849.188850746</v>
       </c>
     </row>
     <row r="1004" spans="1:8">
@@ -29875,11 +29903,11 @@
       </c>
       <c r="G1014" s="1">
         <f t="shared" si="46"/>
-        <v>35711672.73071482</v>
+        <v>43458512.817083389</v>
       </c>
       <c r="H1014" s="1">
         <f t="shared" si="47"/>
-        <v>11330542.26928518</v>
+        <v>3583702.1829166114</v>
       </c>
     </row>
     <row r="1015" spans="1:8">
@@ -30687,11 +30715,11 @@
       </c>
       <c r="G1042" s="1">
         <f t="shared" si="49"/>
-        <v>49085212.946546622</v>
+        <v>59733140.255064882</v>
       </c>
       <c r="H1042" s="1">
         <f t="shared" si="50"/>
-        <v>101320199.05345339</v>
+        <v>90672271.744935125</v>
       </c>
     </row>
     <row r="1043" spans="1:8">
@@ -32166,11 +32194,11 @@
       </c>
       <c r="G1093" s="1">
         <f t="shared" si="52"/>
-        <v>43905202.86335323</v>
+        <v>53429444.085731864</v>
       </c>
       <c r="H1093" s="1">
         <f t="shared" si="53"/>
-        <v>56655922.13664677</v>
+        <v>47131680.914268136</v>
       </c>
     </row>
     <row r="1094" spans="1:8">
@@ -32978,11 +33006,11 @@
       </c>
       <c r="G1121" s="1">
         <f t="shared" si="52"/>
-        <v>15914538.186723329</v>
+        <v>19366837.475827057</v>
       </c>
       <c r="H1121" s="1">
         <f t="shared" si="53"/>
-        <v>6229729.1867233291</v>
+        <v>9682028.4758270569</v>
       </c>
     </row>
     <row r="1122" spans="1:8">
@@ -33297,11 +33325,11 @@
       </c>
       <c r="G1132" s="1">
         <f t="shared" si="52"/>
-        <v>16145198.765279777</v>
+        <v>19647534.652494721</v>
       </c>
       <c r="H1132" s="1">
         <f t="shared" si="53"/>
-        <v>10386680.234720223</v>
+        <v>6884344.3475052789</v>
       </c>
     </row>
     <row r="1133" spans="1:8">
@@ -33326,11 +33354,11 @@
       </c>
       <c r="G1133" s="1">
         <f t="shared" si="52"/>
-        <v>43905202.86335323</v>
+        <v>53429444.085731864</v>
       </c>
       <c r="H1133" s="1">
         <f t="shared" si="53"/>
-        <v>56655922.13664677</v>
+        <v>47131680.914268136</v>
       </c>
     </row>
     <row r="1134" spans="1:8">
@@ -33384,11 +33412,11 @@
       </c>
       <c r="G1135" s="1">
         <f t="shared" si="52"/>
-        <v>38536072.352066725</v>
+        <v>46895602.086764053</v>
       </c>
       <c r="H1135" s="1">
         <f t="shared" si="53"/>
-        <v>64214592.647933275</v>
+        <v>55855062.913235947</v>
       </c>
     </row>
     <row r="1136" spans="1:8">
@@ -33413,11 +33441,11 @@
       </c>
       <c r="G1136" s="1">
         <f t="shared" si="52"/>
-        <v>25750721.440437559</v>
+        <v>31336758.325685956</v>
       </c>
       <c r="H1136" s="1">
         <f t="shared" si="53"/>
-        <v>13038449.440437559</v>
+        <v>18624486.325685956</v>
       </c>
     </row>
     <row r="1137" spans="1:8">
@@ -33500,11 +33528,11 @@
       </c>
       <c r="G1139" s="1">
         <f t="shared" si="52"/>
-        <v>18058486.213907789</v>
+        <v>21975866.560550399</v>
       </c>
       <c r="H1139" s="1">
         <f t="shared" si="53"/>
-        <v>3467073.7860922106</v>
+        <v>450306.56055039912</v>
       </c>
     </row>
     <row r="1140" spans="1:8">
@@ -33616,11 +33644,11 @@
       </c>
       <c r="G1143" s="1">
         <f t="shared" si="52"/>
-        <v>20628858.168314341</v>
+        <v>25103822.603594393</v>
       </c>
       <c r="H1143" s="1">
         <f t="shared" si="53"/>
-        <v>7200986.1683143415</v>
+        <v>11675950.603594393</v>
       </c>
     </row>
     <row r="1144" spans="1:8">
@@ -33703,11 +33731,11 @@
       </c>
       <c r="G1146" s="1">
         <f t="shared" si="52"/>
-        <v>11296845.167399678</v>
+        <v>13747440.345402678</v>
       </c>
       <c r="H1146" s="1">
         <f t="shared" si="53"/>
-        <v>2098764.8326003216</v>
+        <v>351830.34540267847</v>
       </c>
     </row>
     <row r="1147" spans="1:8">
@@ -33769,6 +33797,10 @@
       </c>
     </row>
     <row r="1151" spans="1:8">
+      <c r="D1151" s="1">
+        <f>SUM(D2:D1148)</f>
+        <v>8090967854</v>
+      </c>
       <c r="F1151" s="1">
         <f>SUM(F2:F1148)</f>
         <v>3593747261.1115956</v>
@@ -33776,16 +33808,26 @@
       <c r="G1151" s="1"/>
       <c r="H1151" s="1">
         <f>SUM(H2:H1148)</f>
-        <v>3644200987.8740945</v>
+        <v>3542290997.2638464</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
       <formula>99000000</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThan">
       <formula>100000000</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+      <formula>15000000</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:H1048576">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>15000000</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>